<commit_message>
Add images extracting functionality and refactor some parts of code, not yet finished
</commit_message>
<xml_diff>
--- a/output/page_2.xlsx
+++ b/output/page_2.xlsx
@@ -108,7 +108,28 @@
 500S</t>
   </si>
   <si>
-    <t>3/8</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/8</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C:\Work\Table-extractor\output\page_2_image_1.png</t>
+    </r>
   </si>
   <si>
     <t>SILVERMOON

</xml_diff>